<commit_message>
un par de cambios
</commit_message>
<xml_diff>
--- a/Terminos/Conceptualizacion.xlsx
+++ b/Terminos/Conceptualizacion.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="7995" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Conceptos" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="80">
   <si>
     <t>Diccionario</t>
   </si>
@@ -63,9 +63,6 @@
     <t>jugador</t>
   </si>
   <si>
-    <t>ejecutar el juego</t>
-  </si>
-  <si>
     <t>fielder</t>
   </si>
   <si>
@@ -126,9 +123,6 @@
     <t>forma de soltar la bola al momento de lanzar</t>
   </si>
   <si>
-    <t>postura</t>
-  </si>
-  <si>
     <t>movimiento y postura del cuerpo al momento de lanzar</t>
   </si>
   <si>
@@ -150,19 +144,129 @@
     <t>izquierda, derecha</t>
   </si>
   <si>
-    <t>posicion
-equipo
-postura
+    <t>windup ( de frente ), set (de lado)</t>
+  </si>
+  <si>
+    <t>ejecutar el lanzamiento</t>
+  </si>
+  <si>
+    <t>pitcher</t>
+  </si>
+  <si>
+    <t>posicion cuerpo</t>
+  </si>
+  <si>
+    <t>posicion cuerpo
 agarre
 efecto
-mano</t>
+mano
+distacia brazo-cuerpo</t>
+  </si>
+  <si>
+    <t>velocidad</t>
+  </si>
+  <si>
+    <t>lanzador</t>
+  </si>
+  <si>
+    <t>velocidad que alcanza la bola</t>
+  </si>
+  <si>
+    <t>dirección</t>
+  </si>
+  <si>
+    <t>dirección en la que la bola alcanza el plato</t>
+  </si>
+  <si>
+    <t>derecha, izquierda, centro, arriba, medio, abajo</t>
+  </si>
+  <si>
+    <t>traza</t>
+  </si>
+  <si>
+    <t>recorrido de la bola</t>
+  </si>
+  <si>
+    <t>recto, curva, trepa, baja</t>
+  </si>
+  <si>
+    <t>pueden ser combinables? Cual es el nombre tecnico veritooo?</t>
+  </si>
+  <si>
+    <t>direccion</t>
+  </si>
+  <si>
+    <t>izquierda</t>
+  </si>
+  <si>
+    <t>derecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> izquierda</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> centro</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> arriba</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> medio</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> abajo</t>
+  </si>
+  <si>
+    <t>recto</t>
+  </si>
+  <si>
+    <t>curva</t>
+  </si>
+  <si>
+    <t>trepa</t>
+  </si>
+  <si>
+    <t>baja</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>lenta</t>
+  </si>
+  <si>
+    <t>rapida</t>
+  </si>
+  <si>
+    <t>de frente</t>
+  </si>
+  <si>
+    <t>de lado</t>
+  </si>
+  <si>
+    <t>fastball</t>
+  </si>
+  <si>
+    <t>riseball</t>
+  </si>
+  <si>
+    <t>dropball</t>
+  </si>
+  <si>
+    <t>curveball</t>
+  </si>
+  <si>
+    <t>changeup</t>
+  </si>
+  <si>
+    <t>screwball</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,6 +290,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -195,7 +314,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -203,11 +322,191 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -232,6 +531,82 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -530,133 +905,385 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="1" max="1" width="11.42578125" style="9"/>
     <col min="2" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" s="9" customFormat="1">
+      <c r="A4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="2" customFormat="1" ht="90">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
+    <row r="5" spans="1:6" s="2" customFormat="1" ht="75">
+      <c r="A5" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="36.75" customHeight="1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="2" customFormat="1"/>
-    <row r="8" spans="1:6" s="2" customFormat="1"/>
-    <row r="9" spans="1:6" s="2" customFormat="1"/>
-    <row r="10" spans="1:6" s="2" customFormat="1"/>
-    <row r="11" spans="1:6" s="2" customFormat="1"/>
-    <row r="12" spans="1:6" s="2" customFormat="1"/>
-    <row r="13" spans="1:6" s="2" customFormat="1"/>
-    <row r="14" spans="1:6" s="2" customFormat="1"/>
-    <row r="15" spans="1:6" s="2" customFormat="1"/>
-    <row r="16" spans="1:6" s="2" customFormat="1"/>
-    <row r="17" s="2" customFormat="1"/>
-    <row r="18" s="2" customFormat="1"/>
-    <row r="19" s="2" customFormat="1"/>
-    <row r="20" s="2" customFormat="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="2" customFormat="1">
+      <c r="A7" s="10"/>
+    </row>
+    <row r="8" spans="1:6" s="2" customFormat="1">
+      <c r="A8" s="10"/>
+    </row>
+    <row r="9" spans="1:6" s="2" customFormat="1">
+      <c r="A9" s="10"/>
+    </row>
+    <row r="10" spans="1:6" s="2" customFormat="1">
+      <c r="A10" s="10"/>
+    </row>
+    <row r="11" spans="1:6" s="2" customFormat="1">
+      <c r="A11" s="10"/>
+    </row>
+    <row r="12" spans="1:6" s="2" customFormat="1">
+      <c r="A12" s="10"/>
+    </row>
+    <row r="13" spans="1:6" s="2" customFormat="1">
+      <c r="A13" s="10"/>
+    </row>
+    <row r="14" spans="1:6" s="2" customFormat="1">
+      <c r="A14" s="10"/>
+    </row>
+    <row r="15" spans="1:6" s="2" customFormat="1">
+      <c r="A15" s="10"/>
+    </row>
+    <row r="16" spans="1:6" s="2" customFormat="1">
+      <c r="A16" s="10"/>
+    </row>
+    <row r="17" spans="1:1" s="2" customFormat="1">
+      <c r="A17" s="10"/>
+    </row>
+    <row r="18" spans="1:1" s="2" customFormat="1">
+      <c r="A18" s="10"/>
+    </row>
+    <row r="19" spans="1:1" s="2" customFormat="1">
+      <c r="A19" s="10"/>
+    </row>
+    <row r="20" spans="1:1" s="2" customFormat="1">
+      <c r="A20" s="10"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:C3"/>
+  <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="16" customWidth="1"/>
+    <col min="4" max="16384" width="11.42578125" style="16"/>
+  </cols>
   <sheetData>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
+    <row r="2" spans="1:7" ht="15.75" thickBot="1"/>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="24" t="s">
         <v>8</v>
       </c>
     </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="27"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="28"/>
+      <c r="B5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="29"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="28"/>
+      <c r="B6" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="30"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="28"/>
+      <c r="B7" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="28"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="29" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="28"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="28"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="28"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="29" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="28"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="28"/>
+      <c r="B13" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="28"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="G14" s="17"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="28"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="G15" s="18"/>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="28"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="29" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="28"/>
+      <c r="B17" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="28"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="29" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="28"/>
+      <c r="B19" s="19"/>
+      <c r="C19" s="29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="28"/>
+      <c r="B20" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="28"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="29" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="28"/>
+      <c r="B22" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="28"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="28"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="28"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="28"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="31" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="28"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A29" s="32"/>
+      <c r="B29" s="33"/>
+      <c r="C29" s="34" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A24:A29"/>
+    <mergeCell ref="A4:A23"/>
+    <mergeCell ref="B7:B12"/>
+    <mergeCell ref="B13:B16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B29"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:H16"/>
+  <dimension ref="A3:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -688,176 +1315,213 @@
         <v>11</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="H3" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="12" customFormat="1" ht="88.5" customHeight="1">
+      <c r="A4" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="14">
+        <v>1</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" s="12" customFormat="1" ht="45">
+      <c r="A5" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="14">
+        <v>1</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="15" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" ht="88.5" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" s="2" customFormat="1" ht="45">
-      <c r="A5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" s="2" customFormat="1" ht="45">
       <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>32</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" ht="45">
       <c r="A7" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" ht="45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="30">
       <c r="A8" s="7" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>51</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" ht="30">
+      <c r="F8" s="4">
+        <v>2</v>
+      </c>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1">
       <c r="A9" s="7" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4">
+        <v>2</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1">
+      <c r="A10" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" s="2" customFormat="1" ht="45">
+      <c r="A11" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" ht="45">
-      <c r="A10" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" s="2" customFormat="1">
-      <c r="A11" s="7"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" s="2" customFormat="1">
-      <c r="A12" s="7"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="2" customFormat="1" ht="30">
+      <c r="A12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1">
-      <c r="A13" s="7"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" ht="45">
+      <c r="A13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:8" s="2" customFormat="1">
       <c r="A14" s="7"/>
@@ -880,6 +1544,27 @@
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
     </row>
+    <row r="17" spans="1:6" s="2" customFormat="1">
+      <c r="A17" s="7"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1">
+      <c r="A18" s="7"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1">
+      <c r="A19" s="7"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>